<commit_message>
Cronograma de Atividades - BullkApp
</commit_message>
<xml_diff>
--- a/gestao_projetos/Cronograma.xlsx
+++ b/gestao_projetos/Cronograma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\ProjetoIntegrador\gestao_projetos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115DEC29-AF00-4D09-A0E1-BA447644152C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280AF3DF-E934-417F-91FD-E353CC9383B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="4310" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>leoal</author>
+  </authors>
+  <commentList>
+    <comment ref="A34" authorId="0" shapeId="0" xr:uid="{C0C6679D-D538-4B91-9ACC-291D311E0562}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Leonardo Almeida:
+Não está seguindo a ordem da EAP, visto que ela se está incorreta.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>BullkApp</t>
   </si>
@@ -87,38 +122,119 @@
     <t>1.1.6 Cronograma do Projeto</t>
   </si>
   <si>
-    <t>2.1.1 Definição do Projeto</t>
-  </si>
-  <si>
-    <t>2.1.2 Definição do Nome</t>
-  </si>
-  <si>
-    <t>2.1.3 Definição das Tecnologias</t>
-  </si>
-  <si>
-    <t>2.2.1 Apresentação Ideia para a Banca</t>
-  </si>
-  <si>
-    <t>2.2.2 Apresentação Documento de Requisitos para a Banca</t>
-  </si>
-  <si>
-    <t>2.2.3 Apresentação Documento Caso de Uso para a Banca</t>
-  </si>
-  <si>
-    <t>2.2.4 Apresentação Final do Projeto para a Banca</t>
-  </si>
-  <si>
-    <t>3.1.1 Especificação de Requisitos</t>
-  </si>
-  <si>
     <t>7.Desenvolver Registro de Stakeholders</t>
+  </si>
+  <si>
+    <t>8.Revisar Atividades da EAP</t>
+  </si>
+  <si>
+    <t>9.Definição dos prazos para as atividades</t>
+  </si>
+  <si>
+    <t>10.Criação do Cronograma</t>
+  </si>
+  <si>
+    <t>2.1.1 Especificação de Requisitos</t>
+  </si>
+  <si>
+    <t>11.Levantamento dos Requisitos do Sistema</t>
+  </si>
+  <si>
+    <t>2.1.2 Especificação Caso de Uso</t>
+  </si>
+  <si>
+    <t>14.Desenvolver Documento Caso de Uso</t>
+  </si>
+  <si>
+    <t>15.Revisão Documento Caso de Uso</t>
+  </si>
+  <si>
+    <t>12.Desenvolver Documento Especificação de Requisito</t>
+  </si>
+  <si>
+    <t>13.Revisão Documento Especificação de Requisito</t>
+  </si>
+  <si>
+    <t>2.1.3 Diagrama de Classe</t>
+  </si>
+  <si>
+    <t>16.Desenvolver Diagrama de Classe</t>
+  </si>
+  <si>
+    <t>17.Revisão Diagrama de Classe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.Desenvolver Protótipos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.Revisão Protótipos </t>
+  </si>
+  <si>
+    <t>2.2.1 Apresentação Ideia para Banca</t>
+  </si>
+  <si>
+    <t>2.1.4 Prototipação</t>
+  </si>
+  <si>
+    <t>20.Levantamento necessidades do Mercado</t>
+  </si>
+  <si>
+    <t>21.Definição da Ideia</t>
+  </si>
+  <si>
+    <t>2.2.2 Apresentação Documentação de Requisito Para a Banca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.Organização da Documentação de Requisitos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.Organização da Documentação Caso de Uso </t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.Organização da Documentação Caso de Uso </t>
+  </si>
+  <si>
+    <t>2.2.3 Apresentação Documentação de Caso de Uso Para a Banca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.Revisão da Documentação de Requisitos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.Revisão da Documentação Caso de Uso </t>
+  </si>
+  <si>
+    <t>2.2.4 Apresentação Final do Projeto Para a Banca</t>
+  </si>
+  <si>
+    <t>3.2.2 Codificação</t>
+  </si>
+  <si>
+    <t>4.0 Teste do Sistema</t>
+  </si>
+  <si>
+    <t>32.Realização dos Testes do Sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.Organização da Documentação de Requisitos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.Organização da Documentação Caso de Uso </t>
+  </si>
+  <si>
+    <t>29.Cursos/Capacitação</t>
+  </si>
+  <si>
+    <t>30.Codificação</t>
+  </si>
+  <si>
+    <t>31.Revisão da Codificação da Aplicação</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +287,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -180,7 +309,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -274,30 +403,6 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
       <right/>
       <top style="medium">
         <color rgb="FF000000"/>
@@ -332,6 +437,19 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -341,74 +459,79 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -689,87 +812,88 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A15"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="60" customWidth="1"/>
-    <col min="2" max="2" width="52.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.54296875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.81640625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="62.453125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.90625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:6" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="17"/>
-    </row>
-    <row r="2" spans="1:6" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="18" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" ht="30.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="2" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="3">
         <v>2</v>
       </c>
       <c r="D6" s="9">
@@ -778,14 +902,14 @@
       <c r="E6" s="9">
         <v>45005</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="14"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="20"/>
+      <c r="B7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="3">
         <v>0.5</v>
       </c>
       <c r="D7" s="9">
@@ -794,18 +918,18 @@
       <c r="E7" s="9">
         <v>45005</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="3">
         <v>2</v>
       </c>
       <c r="D8" s="9">
@@ -814,16 +938,16 @@
       <c r="E8" s="9">
         <v>45017</v>
       </c>
-      <c r="F8" s="10"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="3">
         <v>2</v>
       </c>
       <c r="D9" s="9">
@@ -832,14 +956,14 @@
       <c r="E9" s="9">
         <v>45018</v>
       </c>
-      <c r="F9" s="10"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="14"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="3">
         <v>0.5</v>
       </c>
       <c r="D10" s="9">
@@ -848,19 +972,19 @@
       <c r="E10" s="9">
         <v>45018</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="10">
-        <v>2</v>
+      <c r="C11" s="3">
+        <v>1.5</v>
       </c>
       <c r="D11" s="9">
         <v>45018</v>
@@ -868,16 +992,16 @@
       <c r="E11" s="9">
         <v>45018</v>
       </c>
-      <c r="F11" s="10"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="10">
+      <c r="B12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3">
         <v>2</v>
       </c>
       <c r="D12" s="9">
@@ -886,241 +1010,471 @@
       <c r="E12" s="9">
         <v>45028</v>
       </c>
-      <c r="F12" s="10"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
+      <c r="B13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="9">
+        <v>45026</v>
+      </c>
+      <c r="E13" s="9">
+        <v>45026</v>
+      </c>
+      <c r="F13" s="3">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="13"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9">
+        <v>45031</v>
+      </c>
+      <c r="E14" s="9">
+        <v>45031</v>
+      </c>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="14"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9">
+        <v>45031</v>
+      </c>
+      <c r="E15" s="9">
+        <v>45031</v>
+      </c>
+      <c r="F15" s="3">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="3">
+        <v>3</v>
+      </c>
+      <c r="D16" s="9">
+        <v>44992</v>
+      </c>
+      <c r="E16" s="9">
+        <v>44992</v>
+      </c>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="20"/>
+      <c r="B17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="3">
+        <v>3</v>
+      </c>
+      <c r="D17" s="9">
+        <v>45003</v>
+      </c>
+      <c r="E17" s="9">
+        <v>45003</v>
+      </c>
+      <c r="F17" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="20"/>
+      <c r="B18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9">
+        <v>45020</v>
+      </c>
+      <c r="E18" s="9">
+        <v>45020</v>
+      </c>
+      <c r="F18" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3">
+        <v>4</v>
+      </c>
+      <c r="D19" s="9">
+        <v>45017</v>
+      </c>
+      <c r="E19" s="9">
+        <v>45071</v>
+      </c>
+      <c r="F19" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="20"/>
+      <c r="B20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="3">
+        <v>3</v>
+      </c>
+      <c r="D20" s="9">
+        <v>45072</v>
+      </c>
+      <c r="E20" s="9">
+        <v>45076</v>
+      </c>
+      <c r="F20" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="9">
+        <v>45069</v>
+      </c>
+      <c r="E21" s="9">
+        <v>45071</v>
+      </c>
+      <c r="F21" s="3">
+        <v>12.14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="20"/>
+      <c r="B22" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1</v>
+      </c>
+      <c r="D22" s="9">
+        <v>45070</v>
+      </c>
+      <c r="E22" s="9">
+        <v>45070</v>
+      </c>
+      <c r="F22" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="3">
+        <v>8</v>
+      </c>
+      <c r="D23" s="9">
+        <v>45003</v>
+      </c>
+      <c r="E23" s="9">
+        <v>45066</v>
+      </c>
+      <c r="F23" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="20"/>
+      <c r="B24" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2</v>
+      </c>
+      <c r="D24" s="9">
+        <v>45070</v>
+      </c>
+      <c r="E24" s="9">
+        <v>45070</v>
+      </c>
+      <c r="F24" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1</v>
+      </c>
+      <c r="D25" s="9">
+        <v>45015</v>
+      </c>
+      <c r="E25" s="9">
+        <v>45015</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="20"/>
+      <c r="B26" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1</v>
+      </c>
+      <c r="D26" s="9">
+        <v>45015</v>
+      </c>
+      <c r="E26" s="9">
+        <v>45015</v>
+      </c>
+      <c r="F26" s="3">
         <v>20</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="13"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-    </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="14"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-    </row>
-    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-    </row>
-    <row r="20" spans="1:6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="13"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-    </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="14"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-    </row>
-    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-    </row>
-    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="13"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-    </row>
-    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="14"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-    </row>
-    <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-    </row>
-    <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="13"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
     </row>
     <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="14"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
+      <c r="A27" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="9">
+        <v>45039</v>
+      </c>
+      <c r="E27" s="9">
+        <v>45039</v>
+      </c>
+      <c r="F27" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="9">
+        <v>45039</v>
+      </c>
+      <c r="E28" s="9">
+        <v>45039</v>
+      </c>
+      <c r="F28" s="3">
+        <v>14</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="13"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
+      <c r="A29" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="9">
+        <v>45089</v>
+      </c>
+      <c r="E29" s="9">
+        <v>45089</v>
+      </c>
+      <c r="F29" s="3">
+        <v>14</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="14"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
+      <c r="A30" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+      <c r="D30" s="9">
+        <v>45254</v>
+      </c>
+      <c r="E30" s="9">
+        <v>45254</v>
+      </c>
+      <c r="F30" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D31" s="9">
+        <v>45255</v>
+      </c>
+      <c r="E31" s="9">
+        <v>45255</v>
+      </c>
+      <c r="F31" s="3">
+        <v>14</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="13"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D32" s="9">
+        <v>45256</v>
+      </c>
+      <c r="E32" s="9">
+        <v>45256</v>
+      </c>
+      <c r="F32" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="14"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-    </row>
-    <row r="34" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
+      <c r="A33" s="20"/>
+      <c r="B33" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="9">
+        <v>45256</v>
+      </c>
+      <c r="E33" s="9">
+        <v>45256</v>
+      </c>
+      <c r="F33" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="3">
+        <v>50</v>
+      </c>
+      <c r="D34" s="9">
+        <v>45017</v>
+      </c>
+      <c r="E34" s="9">
+        <v>45245</v>
+      </c>
+      <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="13"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
+      <c r="A35" s="20"/>
+      <c r="B35" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="3">
+        <v>120</v>
+      </c>
+      <c r="D35" s="9">
+        <v>45047</v>
+      </c>
+      <c r="E35" s="9">
+        <v>45245</v>
+      </c>
+      <c r="F35" s="3">
+        <v>29</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="14"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-    </row>
-    <row r="37" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-    </row>
-    <row r="38" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="13"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-    </row>
-    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="14"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
+      <c r="A36" s="20"/>
+      <c r="B36" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="3">
+        <v>10</v>
+      </c>
+      <c r="D36" s="9">
+        <v>45139</v>
+      </c>
+      <c r="E36" s="9">
+        <v>45248</v>
+      </c>
+      <c r="F36" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="3">
+        <v>10</v>
+      </c>
+      <c r="D37" s="9">
+        <v>45246</v>
+      </c>
+      <c r="E37" s="9">
+        <v>45256</v>
+      </c>
+      <c r="F37" s="3">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1130,15 +1484,16 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A37:A39"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A30:A33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Criação da planilha referente ao acompanhamento de métricas do projeto
</commit_message>
<xml_diff>
--- a/gestao_projetos/Cronograma.xlsx
+++ b/gestao_projetos/Cronograma.xlsx
@@ -1,24 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\ProjetoIntegrador\gestao_projetos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\ProjetoIntegrador\gestao_projetos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280AF3DF-E934-417F-91FD-E353CC9383B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E63631-32C3-4524-A3F4-15A71810AF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="4310" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -60,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>BullkApp</t>
   </si>
@@ -228,13 +240,49 @@
   </si>
   <si>
     <t>31.Revisão da Codificação da Aplicação</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Concluído</t>
+  </si>
+  <si>
+    <t>A Iniciar</t>
+  </si>
+  <si>
+    <t>Em Andamento</t>
+  </si>
+  <si>
+    <t>Conclusão</t>
+  </si>
+  <si>
+    <t>dias para conclusão</t>
+  </si>
+  <si>
+    <t>horas por dia de conclusão</t>
+  </si>
+  <si>
+    <t>dias que já se passaram</t>
+  </si>
+  <si>
+    <t>Horas que deveriam estar concluidas</t>
+  </si>
+  <si>
+    <t>Horas concluídas</t>
+  </si>
+  <si>
+    <t>Deveria estar concluído</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,6 +348,13 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -309,7 +364,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -321,43 +376,6 @@
       <left style="medium">
         <color rgb="FFCCCCCC"/>
       </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color rgb="FFCCCCCC"/>
       </right>
@@ -400,43 +418,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color rgb="FF000000"/>
@@ -464,22 +445,87 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -491,34 +537,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -527,15 +579,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -812,53 +884,100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7081BF2-331C-4804-BA1B-4AFF21F5B507}">
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="O38" sqref="O38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="62.453125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.90625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="18.54296875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.81640625" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="6"/>
+    <col min="1" max="1" width="62.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.88671875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.77734375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.77734375" style="6"/>
+    <col min="10" max="10" width="14.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.77734375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="16"/>
-    </row>
-    <row r="2" spans="1:6" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="19"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="11"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" spans="1:16" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22"/>
+    </row>
+    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
+    </row>
+    <row r="4" spans="1:16" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
@@ -877,17 +996,43 @@
       <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11"/>
       <c r="B5" s="7"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="20" t="s">
+      <c r="G5" s="1"/>
+      <c r="H5" s="3"/>
+      <c r="J5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -903,9 +1048,41 @@
         <v>45005</v>
       </c>
       <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="20"/>
+      <c r="G6" s="26">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="str">
+        <f>IF(G6=1,"Concluído", IF(G6&gt;0,"Em Andamento","A Iniciar"))</f>
+        <v>Concluído</v>
+      </c>
+      <c r="J6" s="6">
+        <f>G6*C6</f>
+        <v>2</v>
+      </c>
+      <c r="K6" s="6">
+        <f ca="1">IF(E6&lt;=TODAY(),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="L6" s="6">
+        <f>IF(E6-D6=0,1,E6-D6)</f>
+        <v>1</v>
+      </c>
+      <c r="M6" s="6">
+        <f t="shared" ref="M6:M34" si="0">C6/L6</f>
+        <v>2</v>
+      </c>
+      <c r="N6" s="28">
+        <f t="shared" ref="N6:N33" ca="1" si="1">IF(D6&lt;=TODAY(),IF(E6&lt;=TODAY(),L6,TODAY()-D6),0)</f>
+        <v>1</v>
+      </c>
+      <c r="O6" s="6">
+        <f>G6*C6</f>
+        <v>2</v>
+      </c>
+      <c r="P6" s="29"/>
+    </row>
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="15"/>
       <c r="B7" s="10" t="s">
         <v>10</v>
       </c>
@@ -921,9 +1098,41 @@
       <c r="F7" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="21" t="s">
+      <c r="G7" s="26">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3" t="str">
+        <f t="shared" ref="H7:H37" si="2">IF(G7=1,"Concluído", IF(G7&gt;0,"Em Andamento","A Iniciar"))</f>
+        <v>Concluído</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" ref="J7:J37" si="3">G7*C7</f>
+        <v>0.5</v>
+      </c>
+      <c r="K7" s="6">
+        <f t="shared" ref="K7:K37" ca="1" si="4">IF(E7&lt;=TODAY(),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="L7" s="6">
+        <f t="shared" ref="L7:L37" si="5">IF(E7-D7=0,1,E7-D7)</f>
+        <v>1</v>
+      </c>
+      <c r="M7" s="6">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="N7" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O7" s="6">
+        <f t="shared" ref="O6:O37" si="6">G7*C7</f>
+        <v>0.5</v>
+      </c>
+      <c r="P7" s="29"/>
+    </row>
+    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -939,9 +1148,41 @@
         <v>45017</v>
       </c>
       <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="20" t="s">
+      <c r="G8" s="26">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="K8" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L8" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M8" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N8" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O8" s="6">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="P8" s="29"/>
+    </row>
+    <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -957,9 +1198,41 @@
         <v>45018</v>
       </c>
       <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="20"/>
+      <c r="G9" s="26">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="K9" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L9" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M9" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N9" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O9" s="6">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="P9" s="29"/>
+    </row>
+    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="15"/>
       <c r="B10" s="10" t="s">
         <v>15</v>
       </c>
@@ -975,9 +1248,41 @@
       <c r="F10" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="21" t="s">
+      <c r="G10" s="26">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L10" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="N10" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O10" s="6">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="P10" s="29"/>
+    </row>
+    <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -993,9 +1298,41 @@
         <v>45018</v>
       </c>
       <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="21" t="s">
+      <c r="G11" s="26">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J11" s="6">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
+      <c r="K11" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L11" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M11" s="6">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="N11" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O11" s="6">
+        <f t="shared" si="6"/>
+        <v>1.5</v>
+      </c>
+      <c r="P11" s="29"/>
+    </row>
+    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="14" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -1011,9 +1348,41 @@
         <v>45028</v>
       </c>
       <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="20" t="s">
+      <c r="G12" s="26">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J12" s="6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="K12" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L12" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M12" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N12" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O12" s="6">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="P12" s="29"/>
+    </row>
+    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -1031,9 +1400,41 @@
       <c r="F13" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="20"/>
+      <c r="G13" s="26">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J13" s="6">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="K13" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L13" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M13" s="6">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="N13" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O13" s="6">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="P13" s="29"/>
+    </row>
+    <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="15"/>
       <c r="B14" s="10" t="s">
         <v>22</v>
       </c>
@@ -1047,9 +1448,41 @@
         <v>45031</v>
       </c>
       <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="20"/>
+      <c r="G14" s="26">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J14" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M14" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N14" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O14" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P14" s="29"/>
+    </row>
+    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="15"/>
       <c r="B15" s="10" t="s">
         <v>23</v>
       </c>
@@ -1065,9 +1498,41 @@
       <c r="F15" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="20" t="s">
+      <c r="G15" s="26">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J15" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K15" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L15" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M15" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N15" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O15" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P15" s="29"/>
+    </row>
+    <row r="16" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="10" t="s">
@@ -1083,9 +1548,41 @@
         <v>44992</v>
       </c>
       <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="20"/>
+      <c r="G16" s="26">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J16" s="6">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="K16" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L16" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M16" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="N16" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O16" s="6">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="P16" s="29"/>
+    </row>
+    <row r="17" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="15"/>
       <c r="B17" s="10" t="s">
         <v>29</v>
       </c>
@@ -1101,9 +1598,41 @@
       <c r="F17" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="20"/>
+      <c r="G17" s="26">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J17" s="6">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="K17" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L17" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M17" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="N17" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O17" s="6">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="P17" s="29"/>
+    </row>
+    <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="15"/>
       <c r="B18" s="10" t="s">
         <v>30</v>
       </c>
@@ -1119,9 +1648,41 @@
       <c r="F18" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="20" t="s">
+      <c r="G18" s="26">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M18" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N18" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O18" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P18" s="29"/>
+    </row>
+    <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -1139,9 +1700,41 @@
       <c r="F19" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="20"/>
+      <c r="G19" s="26">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J19" s="6">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="K19" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L19" s="6">
+        <f t="shared" si="5"/>
+        <v>54</v>
+      </c>
+      <c r="M19" s="6">
+        <f t="shared" si="0"/>
+        <v>7.407407407407407E-2</v>
+      </c>
+      <c r="N19" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="O19" s="6">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="P19" s="29"/>
+    </row>
+    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="15"/>
       <c r="B20" s="10" t="s">
         <v>28</v>
       </c>
@@ -1157,9 +1750,41 @@
       <c r="F20" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="20" t="s">
+      <c r="G20" s="26">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J20" s="6">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="K20" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L20" s="6">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="M20" s="6">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="N20" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="O20" s="6">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="P20" s="29"/>
+    </row>
+    <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="15" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -1177,9 +1802,41 @@
       <c r="F21" s="3">
         <v>12.14</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="20"/>
+      <c r="G21" s="26">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J21" s="6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="K21" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L21" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="M21" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N21" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="O21" s="6">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="P21" s="29"/>
+    </row>
+    <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="15"/>
       <c r="B22" s="10" t="s">
         <v>33</v>
       </c>
@@ -1195,9 +1852,41 @@
       <c r="F22" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="20" t="s">
+      <c r="G22" s="26">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J22" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K22" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L22" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M22" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N22" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O22" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P22" s="29"/>
+    </row>
+    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="15" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="10" t="s">
@@ -1215,9 +1904,41 @@
       <c r="F23" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="20"/>
+      <c r="G23" s="26">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J23" s="6">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="K23" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L23" s="6">
+        <f t="shared" si="5"/>
+        <v>63</v>
+      </c>
+      <c r="M23" s="6">
+        <f t="shared" si="0"/>
+        <v>0.12698412698412698</v>
+      </c>
+      <c r="N23" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="O23" s="6">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="P23" s="29"/>
+    </row>
+    <row r="24" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="15"/>
       <c r="B24" s="10" t="s">
         <v>35</v>
       </c>
@@ -1233,9 +1954,41 @@
       <c r="F24" s="3">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="20" t="s">
+      <c r="G24" s="26">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J24" s="6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="K24" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L24" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M24" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N24" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O24" s="6">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="P24" s="29"/>
+    </row>
+    <row r="25" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="10" t="s">
@@ -1251,9 +2004,41 @@
         <v>45015</v>
       </c>
       <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="20"/>
+      <c r="G25" s="26">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J25" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K25" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L25" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M25" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N25" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O25" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P25" s="29"/>
+    </row>
+    <row r="26" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="15"/>
       <c r="B26" s="10" t="s">
         <v>39</v>
       </c>
@@ -1269,9 +2054,41 @@
       <c r="F26" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="20" t="s">
+      <c r="G26" s="26">
+        <v>1</v>
+      </c>
+      <c r="H26" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J26" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K26" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L26" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M26" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N26" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O26" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P26" s="29"/>
+    </row>
+    <row r="27" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="15" t="s">
         <v>40</v>
       </c>
       <c r="B27" s="10" t="s">
@@ -1289,9 +2106,41 @@
       <c r="F27" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="20"/>
+      <c r="G27" s="26">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J27" s="6">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="K27" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L27" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M27" s="6">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="N27" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O27" s="6">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="P27" s="29"/>
+    </row>
+    <row r="28" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="15"/>
       <c r="B28" s="10" t="s">
         <v>42</v>
       </c>
@@ -1307,9 +2156,41 @@
       <c r="F28" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="21" t="s">
+      <c r="G28" s="26">
+        <v>1</v>
+      </c>
+      <c r="H28" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J28" s="6">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="K28" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L28" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M28" s="6">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="N28" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O28" s="6">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="P28" s="29"/>
+    </row>
+    <row r="29" spans="1:16" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="14" t="s">
         <v>44</v>
       </c>
       <c r="B29" s="10" t="s">
@@ -1327,9 +2208,41 @@
       <c r="F29" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="20" t="s">
+      <c r="G29" s="26">
+        <v>1</v>
+      </c>
+      <c r="H29" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Concluído</v>
+      </c>
+      <c r="J29" s="6">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="K29" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L29" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M29" s="6">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="N29" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O29" s="6">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="P29" s="29"/>
+    </row>
+    <row r="30" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="15" t="s">
         <v>47</v>
       </c>
       <c r="B30" s="10" t="s">
@@ -1347,9 +2260,41 @@
       <c r="F30" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="20"/>
+      <c r="G30" s="26">
+        <v>0</v>
+      </c>
+      <c r="H30" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>A Iniciar</v>
+      </c>
+      <c r="J30" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M30" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N30" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O30" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P30" s="29"/>
+    </row>
+    <row r="31" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="15"/>
       <c r="B31" s="10" t="s">
         <v>46</v>
       </c>
@@ -1365,9 +2310,41 @@
       <c r="F31" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="20"/>
+      <c r="G31" s="26">
+        <v>0</v>
+      </c>
+      <c r="H31" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>A Iniciar</v>
+      </c>
+      <c r="J31" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L31" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M31" s="6">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="N31" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O31" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P31" s="29"/>
+    </row>
+    <row r="32" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="15"/>
       <c r="B32" s="10" t="s">
         <v>51</v>
       </c>
@@ -1383,9 +2360,41 @@
       <c r="F32" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="20"/>
+      <c r="G32" s="26">
+        <v>0</v>
+      </c>
+      <c r="H32" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>A Iniciar</v>
+      </c>
+      <c r="J32" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L32" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M32" s="6">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="N32" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O32" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P32" s="29"/>
+    </row>
+    <row r="33" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="15"/>
       <c r="B33" s="10" t="s">
         <v>52</v>
       </c>
@@ -1401,9 +2410,41 @@
       <c r="F33" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="20" t="s">
+      <c r="G33" s="26">
+        <v>0</v>
+      </c>
+      <c r="H33" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>A Iniciar</v>
+      </c>
+      <c r="J33" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L33" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M33" s="6">
+        <f>C33/L33</f>
+        <v>0.5</v>
+      </c>
+      <c r="N33" s="28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O33" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P33" s="29"/>
+    </row>
+    <row r="34" spans="1:17" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="15" t="s">
         <v>48</v>
       </c>
       <c r="B34" s="10" t="s">
@@ -1419,9 +2460,42 @@
         <v>45245</v>
       </c>
       <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="20"/>
+      <c r="G34" s="26">
+        <v>0.7</v>
+      </c>
+      <c r="H34" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Em Andamento</v>
+      </c>
+      <c r="J34" s="6">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="K34" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L34" s="6">
+        <f t="shared" si="5"/>
+        <v>228</v>
+      </c>
+      <c r="M34" s="6">
+        <f>C34/L34</f>
+        <v>0.21929824561403508</v>
+      </c>
+      <c r="N34" s="28">
+        <f ca="1">IF(D34&lt;=TODAY(),IF(E34&lt;=TODAY(),L34,TODAY()-D34),0)</f>
+        <v>148</v>
+      </c>
+      <c r="O34" s="29">
+        <f ca="1">N34*M34</f>
+        <v>32.456140350877192</v>
+      </c>
+      <c r="P34" s="29"/>
+      <c r="Q34" s="6"/>
+    </row>
+    <row r="35" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="15"/>
       <c r="B35" s="10" t="s">
         <v>54</v>
       </c>
@@ -1437,9 +2511,41 @@
       <c r="F35" s="3">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="20"/>
+      <c r="G35" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="H35" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Em Andamento</v>
+      </c>
+      <c r="J35" s="6">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="K35" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L35" s="6">
+        <f t="shared" ref="L35:L37" si="7">IF(E35-D35=0,1,E35-D35)</f>
+        <v>198</v>
+      </c>
+      <c r="M35" s="6">
+        <f t="shared" ref="M35:M37" si="8">C35/L35</f>
+        <v>0.60606060606060608</v>
+      </c>
+      <c r="N35" s="28">
+        <f t="shared" ref="N35:N37" ca="1" si="9">IF(D35&lt;=TODAY(),IF(E35&lt;=TODAY(),L35,TODAY()-D35),0)</f>
+        <v>118</v>
+      </c>
+      <c r="O35" s="29">
+        <f t="shared" ref="O35:O37" ca="1" si="10">N35*M35</f>
+        <v>71.515151515151516</v>
+      </c>
+      <c r="P35" s="29"/>
+    </row>
+    <row r="36" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="15"/>
       <c r="B36" s="10" t="s">
         <v>55</v>
       </c>
@@ -1455,9 +2561,40 @@
       <c r="F36" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="21" t="s">
+      <c r="G36" s="26">
+        <v>0</v>
+      </c>
+      <c r="H36" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>A Iniciar</v>
+      </c>
+      <c r="J36" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K36" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="6">
+        <f t="shared" si="7"/>
+        <v>109</v>
+      </c>
+      <c r="M36" s="6">
+        <f t="shared" si="8"/>
+        <v>9.1743119266055051E-2</v>
+      </c>
+      <c r="N36" s="28">
+        <f t="shared" ca="1" si="9"/>
+        <v>26</v>
+      </c>
+      <c r="O36" s="29">
+        <f t="shared" ca="1" si="10"/>
+        <v>2.3853211009174311</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="14" t="s">
         <v>49</v>
       </c>
       <c r="B37" s="10" t="s">
@@ -1475,14 +2612,68 @@
       <c r="F37" s="3">
         <v>30</v>
       </c>
+      <c r="G37" s="26">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>A Iniciar</v>
+      </c>
+      <c r="J37" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K37" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L37" s="6">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="M37" s="6">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N37" s="28">
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O37" s="29">
+        <f t="shared" ca="1" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Q37" s="6"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C38" s="5">
+        <f>SUM(C6:C37)</f>
+        <v>237</v>
+      </c>
+      <c r="H38" s="27"/>
+      <c r="J38" s="6">
+        <f>SUM(J6:J37)</f>
+        <v>138.5</v>
+      </c>
+      <c r="O38" s="6">
+        <f ca="1">SUM(O6:O37)</f>
+        <v>149.85661296694613</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M39" s="6">
+        <f>J38/C38</f>
+        <v>0.58438818565400841</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M40" s="6">
+        <f ca="1">J38/O38</f>
+        <v>0.92421680470349976</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A9:A10"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A19:A20"/>
@@ -1491,6 +2682,11 @@
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajustes pontuais referentes à aplicação
</commit_message>
<xml_diff>
--- a/gestao_projetos/Cronograma.xlsx
+++ b/gestao_projetos/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\ProjetoIntegrador\gestao_projetos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E63631-32C3-4524-A3F4-15A71810AF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F96E9F-DD15-4811-A3DA-30816FAB41AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -558,21 +558,33 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -590,18 +602,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -915,12 +915,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q40"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="O38" sqref="O38"/>
+      <selection pane="bottomLeft" activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -944,38 +944,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25"/>
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:16" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
+      <c r="A2" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:16" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
@@ -1032,7 +1032,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -1048,7 +1048,7 @@
         <v>45005</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="26">
+      <c r="G6" s="19">
         <v>1</v>
       </c>
       <c r="H6" s="3" t="str">
@@ -1068,10 +1068,10 @@
         <v>1</v>
       </c>
       <c r="M6" s="6">
-        <f t="shared" ref="M6:M34" si="0">C6/L6</f>
+        <f t="shared" ref="M6:M32" si="0">C6/L6</f>
         <v>2</v>
       </c>
-      <c r="N6" s="28">
+      <c r="N6" s="21">
         <f t="shared" ref="N6:N33" ca="1" si="1">IF(D6&lt;=TODAY(),IF(E6&lt;=TODAY(),L6,TODAY()-D6),0)</f>
         <v>1</v>
       </c>
@@ -1079,10 +1079,10 @@
         <f>G6*C6</f>
         <v>2</v>
       </c>
-      <c r="P6" s="29"/>
+      <c r="P6" s="22"/>
     </row>
     <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="15"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="10" t="s">
         <v>10</v>
       </c>
@@ -1098,7 +1098,7 @@
       <c r="F7" s="3">
         <v>1</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="19">
         <v>1</v>
       </c>
       <c r="H7" s="3" t="str">
@@ -1114,22 +1114,22 @@
         <v>1</v>
       </c>
       <c r="L7" s="6">
-        <f t="shared" ref="L7:L37" si="5">IF(E7-D7=0,1,E7-D7)</f>
+        <f t="shared" ref="L7:L34" si="5">IF(E7-D7=0,1,E7-D7)</f>
         <v>1</v>
       </c>
       <c r="M7" s="6">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="N7" s="28">
+      <c r="N7" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="O7" s="6">
-        <f t="shared" ref="O6:O37" si="6">G7*C7</f>
-        <v>0.5</v>
-      </c>
-      <c r="P7" s="29"/>
+        <f t="shared" ref="O7:O33" si="6">G7*C7</f>
+        <v>0.5</v>
+      </c>
+      <c r="P7" s="22"/>
     </row>
     <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
@@ -1148,7 +1148,7 @@
         <v>45017</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="26">
+      <c r="G8" s="19">
         <v>1</v>
       </c>
       <c r="H8" s="3" t="str">
@@ -1171,7 +1171,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="N8" s="28">
+      <c r="N8" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -1179,10 +1179,10 @@
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="P8" s="29"/>
+      <c r="P8" s="22"/>
     </row>
     <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -1198,7 +1198,7 @@
         <v>45018</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="26">
+      <c r="G9" s="19">
         <v>1</v>
       </c>
       <c r="H9" s="3" t="str">
@@ -1221,7 +1221,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="N9" s="28">
+      <c r="N9" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -1229,10 +1229,10 @@
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="P9" s="29"/>
+      <c r="P9" s="22"/>
     </row>
     <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="10" t="s">
         <v>15</v>
       </c>
@@ -1248,7 +1248,7 @@
       <c r="F10" s="3">
         <v>4</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="19">
         <v>1</v>
       </c>
       <c r="H10" s="3" t="str">
@@ -1271,7 +1271,7 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="N10" s="28">
+      <c r="N10" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -1279,7 +1279,7 @@
         <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="P10" s="29"/>
+      <c r="P10" s="22"/>
     </row>
     <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
@@ -1298,7 +1298,7 @@
         <v>45018</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="26">
+      <c r="G11" s="19">
         <v>1</v>
       </c>
       <c r="H11" s="3" t="str">
@@ -1321,7 +1321,7 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="N11" s="28">
+      <c r="N11" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -1329,7 +1329,7 @@
         <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
-      <c r="P11" s="29"/>
+      <c r="P11" s="22"/>
     </row>
     <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
@@ -1348,7 +1348,7 @@
         <v>45028</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="26">
+      <c r="G12" s="19">
         <v>1</v>
       </c>
       <c r="H12" s="3" t="str">
@@ -1371,7 +1371,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="N12" s="28">
+      <c r="N12" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -1379,10 +1379,10 @@
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="P12" s="29"/>
+      <c r="P12" s="22"/>
     </row>
     <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -1400,7 +1400,7 @@
       <c r="F13" s="3">
         <v>6</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G13" s="19">
         <v>1</v>
       </c>
       <c r="H13" s="3" t="str">
@@ -1423,7 +1423,7 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="N13" s="28">
+      <c r="N13" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -1431,10 +1431,10 @@
         <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="P13" s="29"/>
+      <c r="P13" s="22"/>
     </row>
     <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="15"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="10" t="s">
         <v>22</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>45031</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="26">
+      <c r="G14" s="19">
         <v>1</v>
       </c>
       <c r="H14" s="3" t="str">
@@ -1471,7 +1471,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N14" s="28">
+      <c r="N14" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -1479,10 +1479,10 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="P14" s="29"/>
+      <c r="P14" s="22"/>
     </row>
     <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="15"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="10" t="s">
         <v>23</v>
       </c>
@@ -1498,7 +1498,7 @@
       <c r="F15" s="3">
         <v>9</v>
       </c>
-      <c r="G15" s="26">
+      <c r="G15" s="19">
         <v>1</v>
       </c>
       <c r="H15" s="3" t="str">
@@ -1521,7 +1521,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N15" s="28">
+      <c r="N15" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -1529,10 +1529,10 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="P15" s="29"/>
+      <c r="P15" s="22"/>
     </row>
     <row r="16" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="23" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="10" t="s">
@@ -1548,7 +1548,7 @@
         <v>44992</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="26">
+      <c r="G16" s="19">
         <v>1</v>
       </c>
       <c r="H16" s="3" t="str">
@@ -1571,7 +1571,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="N16" s="28">
+      <c r="N16" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -1579,10 +1579,10 @@
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="P16" s="29"/>
+      <c r="P16" s="22"/>
     </row>
     <row r="17" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="15"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="10" t="s">
         <v>29</v>
       </c>
@@ -1598,7 +1598,7 @@
       <c r="F17" s="3">
         <v>11</v>
       </c>
-      <c r="G17" s="26">
+      <c r="G17" s="19">
         <v>1</v>
       </c>
       <c r="H17" s="3" t="str">
@@ -1621,7 +1621,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="N17" s="28">
+      <c r="N17" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -1629,10 +1629,10 @@
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="P17" s="29"/>
+      <c r="P17" s="22"/>
     </row>
     <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="15"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="10" t="s">
         <v>30</v>
       </c>
@@ -1648,7 +1648,7 @@
       <c r="F18" s="3">
         <v>12</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G18" s="19">
         <v>1</v>
       </c>
       <c r="H18" s="3" t="str">
@@ -1671,7 +1671,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N18" s="28">
+      <c r="N18" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -1679,10 +1679,10 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="P18" s="29"/>
+      <c r="P18" s="22"/>
     </row>
     <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="23" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -1700,7 +1700,7 @@
       <c r="F19" s="3">
         <v>12</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="19">
         <v>1</v>
       </c>
       <c r="H19" s="3" t="str">
@@ -1723,7 +1723,7 @@
         <f t="shared" si="0"/>
         <v>7.407407407407407E-2</v>
       </c>
-      <c r="N19" s="28">
+      <c r="N19" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>54</v>
       </c>
@@ -1731,10 +1731,10 @@
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="P19" s="29"/>
+      <c r="P19" s="22"/>
     </row>
     <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="15"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="10" t="s">
         <v>28</v>
       </c>
@@ -1750,7 +1750,7 @@
       <c r="F20" s="3">
         <v>14</v>
       </c>
-      <c r="G20" s="26">
+      <c r="G20" s="19">
         <v>1</v>
       </c>
       <c r="H20" s="3" t="str">
@@ -1773,7 +1773,7 @@
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="N20" s="28">
+      <c r="N20" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>4</v>
       </c>
@@ -1781,10 +1781,10 @@
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="P20" s="29"/>
+      <c r="P20" s="22"/>
     </row>
     <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="23" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -1802,7 +1802,7 @@
       <c r="F21" s="3">
         <v>12.14</v>
       </c>
-      <c r="G21" s="26">
+      <c r="G21" s="19">
         <v>1</v>
       </c>
       <c r="H21" s="3" t="str">
@@ -1825,7 +1825,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N21" s="28">
+      <c r="N21" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>2</v>
       </c>
@@ -1833,10 +1833,10 @@
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="P21" s="29"/>
+      <c r="P21" s="22"/>
     </row>
     <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="15"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="10" t="s">
         <v>33</v>
       </c>
@@ -1852,7 +1852,7 @@
       <c r="F22" s="3">
         <v>16</v>
       </c>
-      <c r="G22" s="26">
+      <c r="G22" s="19">
         <v>1</v>
       </c>
       <c r="H22" s="3" t="str">
@@ -1875,7 +1875,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N22" s="28">
+      <c r="N22" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -1883,10 +1883,10 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="P22" s="29"/>
+      <c r="P22" s="22"/>
     </row>
     <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="23" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="10" t="s">
@@ -1904,7 +1904,7 @@
       <c r="F23" s="3">
         <v>12</v>
       </c>
-      <c r="G23" s="26">
+      <c r="G23" s="19">
         <v>1</v>
       </c>
       <c r="H23" s="3" t="str">
@@ -1927,7 +1927,7 @@
         <f t="shared" si="0"/>
         <v>0.12698412698412698</v>
       </c>
-      <c r="N23" s="28">
+      <c r="N23" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>63</v>
       </c>
@@ -1935,10 +1935,10 @@
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="P23" s="29"/>
+      <c r="P23" s="22"/>
     </row>
     <row r="24" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="15"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="10" t="s">
         <v>35</v>
       </c>
@@ -1954,7 +1954,7 @@
       <c r="F24" s="3">
         <v>18</v>
       </c>
-      <c r="G24" s="26">
+      <c r="G24" s="19">
         <v>1</v>
       </c>
       <c r="H24" s="3" t="str">
@@ -1977,7 +1977,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="N24" s="28">
+      <c r="N24" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -1985,10 +1985,10 @@
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="P24" s="29"/>
+      <c r="P24" s="22"/>
     </row>
     <row r="25" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="23" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="10" t="s">
@@ -2004,7 +2004,7 @@
         <v>45015</v>
       </c>
       <c r="F25" s="3"/>
-      <c r="G25" s="26">
+      <c r="G25" s="19">
         <v>1</v>
       </c>
       <c r="H25" s="3" t="str">
@@ -2027,7 +2027,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N25" s="28">
+      <c r="N25" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -2035,10 +2035,10 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="P25" s="29"/>
+      <c r="P25" s="22"/>
     </row>
     <row r="26" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="15"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="10" t="s">
         <v>39</v>
       </c>
@@ -2054,7 +2054,7 @@
       <c r="F26" s="3">
         <v>20</v>
       </c>
-      <c r="G26" s="26">
+      <c r="G26" s="19">
         <v>1</v>
       </c>
       <c r="H26" s="3" t="str">
@@ -2077,7 +2077,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N26" s="28">
+      <c r="N26" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -2085,10 +2085,10 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="P26" s="29"/>
+      <c r="P26" s="22"/>
     </row>
     <row r="27" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="23" t="s">
         <v>40</v>
       </c>
       <c r="B27" s="10" t="s">
@@ -2106,7 +2106,7 @@
       <c r="F27" s="3">
         <v>12</v>
       </c>
-      <c r="G27" s="26">
+      <c r="G27" s="19">
         <v>1</v>
       </c>
       <c r="H27" s="3" t="str">
@@ -2129,7 +2129,7 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="N27" s="28">
+      <c r="N27" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -2137,10 +2137,10 @@
         <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="P27" s="29"/>
+      <c r="P27" s="22"/>
     </row>
     <row r="28" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="15"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="10" t="s">
         <v>42</v>
       </c>
@@ -2156,7 +2156,7 @@
       <c r="F28" s="3">
         <v>14</v>
       </c>
-      <c r="G28" s="26">
+      <c r="G28" s="19">
         <v>1</v>
       </c>
       <c r="H28" s="3" t="str">
@@ -2179,7 +2179,7 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="N28" s="28">
+      <c r="N28" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -2187,7 +2187,7 @@
         <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="P28" s="29"/>
+      <c r="P28" s="22"/>
     </row>
     <row r="29" spans="1:16" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="14" t="s">
@@ -2208,7 +2208,7 @@
       <c r="F29" s="3">
         <v>14</v>
       </c>
-      <c r="G29" s="26">
+      <c r="G29" s="19">
         <v>1</v>
       </c>
       <c r="H29" s="3" t="str">
@@ -2231,7 +2231,7 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="N29" s="28">
+      <c r="N29" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
@@ -2239,10 +2239,10 @@
         <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="P29" s="29"/>
+      <c r="P29" s="22"/>
     </row>
     <row r="30" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B30" s="10" t="s">
@@ -2260,7 +2260,7 @@
       <c r="F30" s="3">
         <v>12</v>
       </c>
-      <c r="G30" s="26">
+      <c r="G30" s="19">
         <v>0</v>
       </c>
       <c r="H30" s="3" t="str">
@@ -2283,7 +2283,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N30" s="28">
+      <c r="N30" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
@@ -2291,10 +2291,10 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P30" s="29"/>
+      <c r="P30" s="22"/>
     </row>
     <row r="31" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="15"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="10" t="s">
         <v>46</v>
       </c>
@@ -2310,7 +2310,7 @@
       <c r="F31" s="3">
         <v>14</v>
       </c>
-      <c r="G31" s="26">
+      <c r="G31" s="19">
         <v>0</v>
       </c>
       <c r="H31" s="3" t="str">
@@ -2333,7 +2333,7 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="N31" s="28">
+      <c r="N31" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
@@ -2341,10 +2341,10 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P31" s="29"/>
+      <c r="P31" s="22"/>
     </row>
     <row r="32" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="15"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="10" t="s">
         <v>51</v>
       </c>
@@ -2360,7 +2360,7 @@
       <c r="F32" s="3">
         <v>12</v>
       </c>
-      <c r="G32" s="26">
+      <c r="G32" s="19">
         <v>0</v>
       </c>
       <c r="H32" s="3" t="str">
@@ -2383,7 +2383,7 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="N32" s="28">
+      <c r="N32" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
@@ -2391,10 +2391,10 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P32" s="29"/>
+      <c r="P32" s="22"/>
     </row>
     <row r="33" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="15"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="10" t="s">
         <v>52</v>
       </c>
@@ -2410,7 +2410,7 @@
       <c r="F33" s="3">
         <v>14</v>
       </c>
-      <c r="G33" s="26">
+      <c r="G33" s="19">
         <v>0</v>
       </c>
       <c r="H33" s="3" t="str">
@@ -2433,7 +2433,7 @@
         <f>C33/L33</f>
         <v>0.5</v>
       </c>
-      <c r="N33" s="28">
+      <c r="N33" s="21">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
@@ -2441,10 +2441,10 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P33" s="29"/>
+      <c r="P33" s="22"/>
     </row>
     <row r="34" spans="1:17" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="23" t="s">
         <v>48</v>
       </c>
       <c r="B34" s="10" t="s">
@@ -2460,7 +2460,7 @@
         <v>45245</v>
       </c>
       <c r="F34" s="3"/>
-      <c r="G34" s="26">
+      <c r="G34" s="19">
         <v>0.7</v>
       </c>
       <c r="H34" s="3" t="str">
@@ -2483,19 +2483,19 @@
         <f>C34/L34</f>
         <v>0.21929824561403508</v>
       </c>
-      <c r="N34" s="28">
+      <c r="N34" s="21">
         <f ca="1">IF(D34&lt;=TODAY(),IF(E34&lt;=TODAY(),L34,TODAY()-D34),0)</f>
-        <v>148</v>
-      </c>
-      <c r="O34" s="29">
+        <v>150</v>
+      </c>
+      <c r="O34" s="22">
         <f ca="1">N34*M34</f>
-        <v>32.456140350877192</v>
-      </c>
-      <c r="P34" s="29"/>
+        <v>32.89473684210526</v>
+      </c>
+      <c r="P34" s="22"/>
       <c r="Q34" s="6"/>
     </row>
     <row r="35" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="15"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="10" t="s">
         <v>54</v>
       </c>
@@ -2511,7 +2511,7 @@
       <c r="F35" s="3">
         <v>29</v>
       </c>
-      <c r="G35" s="26">
+      <c r="G35" s="19">
         <v>0.5</v>
       </c>
       <c r="H35" s="3" t="str">
@@ -2534,18 +2534,18 @@
         <f t="shared" ref="M35:M37" si="8">C35/L35</f>
         <v>0.60606060606060608</v>
       </c>
-      <c r="N35" s="28">
+      <c r="N35" s="21">
         <f t="shared" ref="N35:N37" ca="1" si="9">IF(D35&lt;=TODAY(),IF(E35&lt;=TODAY(),L35,TODAY()-D35),0)</f>
-        <v>118</v>
-      </c>
-      <c r="O35" s="29">
+        <v>120</v>
+      </c>
+      <c r="O35" s="22">
         <f t="shared" ref="O35:O37" ca="1" si="10">N35*M35</f>
-        <v>71.515151515151516</v>
-      </c>
-      <c r="P35" s="29"/>
+        <v>72.727272727272734</v>
+      </c>
+      <c r="P35" s="22"/>
     </row>
     <row r="36" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="15"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="10" t="s">
         <v>55</v>
       </c>
@@ -2561,7 +2561,7 @@
       <c r="F36" s="3">
         <v>30</v>
       </c>
-      <c r="G36" s="26">
+      <c r="G36" s="19">
         <v>0</v>
       </c>
       <c r="H36" s="3" t="str">
@@ -2584,13 +2584,13 @@
         <f t="shared" si="8"/>
         <v>9.1743119266055051E-2</v>
       </c>
-      <c r="N36" s="28">
+      <c r="N36" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>26</v>
-      </c>
-      <c r="O36" s="29">
+        <v>28</v>
+      </c>
+      <c r="O36" s="22">
         <f t="shared" ca="1" si="10"/>
-        <v>2.3853211009174311</v>
+        <v>2.5688073394495414</v>
       </c>
     </row>
     <row r="37" spans="1:17" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2612,7 +2612,7 @@
       <c r="F37" s="3">
         <v>30</v>
       </c>
-      <c r="G37" s="26">
+      <c r="G37" s="19">
         <v>0</v>
       </c>
       <c r="H37" s="3" t="str">
@@ -2635,11 +2635,11 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="N37" s="28">
+      <c r="N37" s="21">
         <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
-      <c r="O37" s="29">
+      <c r="O37" s="22">
         <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
@@ -2650,14 +2650,14 @@
         <f>SUM(C6:C37)</f>
         <v>237</v>
       </c>
-      <c r="H38" s="27"/>
+      <c r="H38" s="20"/>
       <c r="J38" s="6">
         <f>SUM(J6:J37)</f>
         <v>138.5</v>
       </c>
       <c r="O38" s="6">
         <f ca="1">SUM(O6:O37)</f>
-        <v>149.85661296694613</v>
+        <v>151.69081690882754</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
@@ -2669,11 +2669,22 @@
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="M40" s="6">
         <f ca="1">J38/O38</f>
-        <v>0.92421680470349976</v>
+        <v>0.91304142744016092</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N42" s="6">
+        <f>M35*7</f>
+        <v>4.2424242424242422</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A1:H1"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A19:A20"/>
@@ -2682,11 +2693,6 @@
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>